<commit_message>
Updates per feedback in PR
</commit_message>
<xml_diff>
--- a/MVPSt_2023_Feb_Competition/MVPSt_2023_Feb_Competition/ExcelData/Mars-Config.xlsx
+++ b/MVPSt_2023_Feb_Competition/MVPSt_2023_Feb_Competition/ExcelData/Mars-Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\MVP Studio Projects\MVPSt_2023_Feb_Competition\MVPSt_2023_Feb_Competition\MVPSt_2023_Feb_Competition\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65DA7273-9907-4F6E-A6FD-59E0B55D4AF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B57D05C-AE38-40FD-87AE-D54FB7D2D7C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="138" yWindow="2477" windowWidth="9977" windowHeight="7949" xr2:uid="{58A694FC-ECEE-4C97-96D0-6EC920A77260}"/>
+    <workbookView xWindow="484" yWindow="2822" windowWidth="9976" windowHeight="7949" xr2:uid="{58A694FC-ECEE-4C97-96D0-6EC920A77260}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -427,7 +427,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -477,7 +477,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="3">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>